<commit_message>
update adcore modules and templates
</commit_message>
<xml_diff>
--- a/adcore/2020/templates/2020-super-category.xlsx
+++ b/adcore/2020/templates/2020-super-category.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/11411/Dropbox/git/repo/agency/adcore/2020/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D66F94D-EED0-E949-B1F5-362A421E7E35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D5EBF0-FCF1-9D41-99BA-E60917F6B9F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="200" yWindow="660" windowWidth="33200" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="124">
   <si>
     <t>Offer Code</t>
   </si>
@@ -183,9 +183,6 @@
     <t>H1</t>
   </si>
   <si>
-    <t>Section 1 Banner 1</t>
-  </si>
-  <si>
     <t>SEO Html</t>
   </si>
   <si>
@@ -382,6 +379,30 @@
   </si>
   <si>
     <t>2020-third-mod</t>
+  </si>
+  <si>
+    <t>M29</t>
+  </si>
+  <si>
+    <t>M30</t>
+  </si>
+  <si>
+    <t>WXX_XX_XXX_XXXBN0300</t>
+  </si>
+  <si>
+    <t>Banner 3</t>
+  </si>
+  <si>
+    <t>WXX_XX_XXX_XXX03H2</t>
+  </si>
+  <si>
+    <t>H2 1</t>
+  </si>
+  <si>
+    <t>H2 2</t>
+  </si>
+  <si>
+    <t>H2 3</t>
   </si>
 </sst>
 </file>
@@ -431,9 +452,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -453,8 +473,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{97FD37EF-440B-164F-A671-9404BC5B49C2}" name="Table2" displayName="Table2" ref="A1:E29" totalsRowShown="0">
-  <autoFilter ref="A1:E29" xr:uid="{46B822AB-FF4E-B747-B408-B19D12290E92}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{97FD37EF-440B-164F-A671-9404BC5B49C2}" name="Table2" displayName="Table2" ref="A1:E31" totalsRowShown="0">
+  <autoFilter ref="A1:E31" xr:uid="{46B822AB-FF4E-B747-B408-B19D12290E92}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{17C01559-4713-534F-9A9B-549B487B8F5A}" name="Module"/>
     <tableColumn id="2" xr3:uid="{FC851083-6D66-B24A-8460-C785CF4AAE2A}" name="Offer Code"/>
@@ -787,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -816,7 +836,7 @@
         <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -824,7 +844,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
         <v>49</v>
@@ -835,10 +855,10 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -846,10 +866,10 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -857,10 +877,10 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -868,10 +888,10 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -879,10 +899,10 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -890,10 +910,10 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -901,10 +921,10 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -912,10 +932,10 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -923,10 +943,10 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -934,10 +954,10 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -945,10 +965,10 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -956,10 +976,10 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -967,10 +987,10 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -978,10 +998,10 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -989,10 +1009,10 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1000,10 +1020,10 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1011,10 +1031,10 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1022,10 +1042,10 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1033,10 +1053,10 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1044,10 +1064,10 @@
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1055,16 +1075,10 @@
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1072,10 +1086,10 @@
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1083,10 +1097,16 @@
         <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C25" t="s">
         <v>67</v>
+      </c>
+      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1094,10 +1114,10 @@
         <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1105,10 +1125,10 @@
         <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1116,10 +1136,10 @@
         <v>47</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1127,9 +1147,31 @@
         <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1147,7 +1189,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1162,31 +1204,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1195,7 +1237,7 @@
         <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -1203,470 +1245,496 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="G3" t="s">
-        <v>116</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" t="s">
         <v>115</v>
-      </c>
-      <c r="C4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
         <v>115</v>
-      </c>
-      <c r="C5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G5" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" t="s">
         <v>115</v>
-      </c>
-      <c r="C6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" t="s">
         <v>115</v>
-      </c>
-      <c r="C7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" t="s">
         <v>115</v>
-      </c>
-      <c r="C8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G8" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" t="s">
         <v>115</v>
-      </c>
-      <c r="C9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G9" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" t="s">
         <v>115</v>
-      </c>
-      <c r="C10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" t="s">
-        <v>95</v>
-      </c>
-      <c r="G10" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" t="s">
+        <v>94</v>
+      </c>
+      <c r="G11" t="s">
         <v>115</v>
-      </c>
-      <c r="C11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" t="s">
-        <v>96</v>
-      </c>
-      <c r="G11" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" t="s">
         <v>115</v>
-      </c>
-      <c r="C12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" t="s">
-        <v>97</v>
-      </c>
-      <c r="G12" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" t="s">
         <v>115</v>
-      </c>
-      <c r="C13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" t="s">
         <v>115</v>
-      </c>
-      <c r="C14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" t="s">
-        <v>99</v>
-      </c>
-      <c r="G14" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="G15" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="G16" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" t="s">
         <v>52</v>
-      </c>
-      <c r="C17" t="s">
-        <v>102</v>
-      </c>
-      <c r="D17" t="s">
-        <v>84</v>
-      </c>
-      <c r="G17" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" t="s">
-        <v>103</v>
-      </c>
-      <c r="D18" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" t="s">
         <v>52</v>
-      </c>
-      <c r="C19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" t="s">
-        <v>86</v>
-      </c>
-      <c r="G19" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" t="s">
         <v>52</v>
-      </c>
-      <c r="C20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="D21" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="D22" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="G22" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G23" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="D24" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="D25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G25" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>119</v>
       </c>
       <c r="D26" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="G26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="D27" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="G27" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" t="s">
         <v>59</v>
       </c>
-      <c r="C29" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" t="s">
-        <v>109</v>
-      </c>
-      <c r="G29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update adcore template .xls file
</commit_message>
<xml_diff>
--- a/adcore/2020/templates/2020-super-category.xlsx
+++ b/adcore/2020/templates/2020-super-category.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/11411/Dropbox/git/repo/agency/adcore/2020/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A02BA5-A587-E94F-9F6E-40CBA7B3157E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537AE3FF-1B91-4246-BF61-6DEB33BAE949}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="660" windowWidth="45780" windowHeight="25500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="45780" windowHeight="25500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CMS" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="126">
   <si>
     <t>Offer Code</t>
   </si>
@@ -201,9 +201,6 @@
     <t xml:space="preserve">W19_00_000_UPLDCTFT </t>
   </si>
   <si>
-    <t xml:space="preserve">W14_00_000_BLKBLNK01 </t>
-  </si>
-  <si>
     <t>W14_00_000_BLKBLNK02</t>
   </si>
   <si>
@@ -403,6 +400,15 @@
   </si>
   <si>
     <t>Accordion List</t>
+  </si>
+  <si>
+    <t>WXX_XX_XXX_XXXBN0400</t>
+  </si>
+  <si>
+    <t>Banner 3/Blank</t>
+  </si>
+  <si>
+    <t>Banner 4</t>
   </si>
 </sst>
 </file>
@@ -810,16 +816,16 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -836,7 +842,7 @@
         <v>37</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -844,7 +850,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
         <v>49</v>
@@ -855,10 +861,10 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -866,10 +872,10 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -877,10 +883,10 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -888,10 +894,10 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -899,10 +905,10 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -910,10 +916,10 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -921,10 +927,10 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -932,10 +938,10 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -943,10 +949,10 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -954,10 +960,10 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -965,10 +971,10 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -976,10 +982,10 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -987,10 +993,10 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -998,10 +1004,10 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1009,10 +1015,10 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1020,10 +1026,10 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1031,10 +1037,10 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1042,10 +1048,10 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1053,10 +1059,10 @@
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1064,10 +1070,10 @@
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1075,10 +1081,10 @@
         <v>42</v>
       </c>
       <c r="B23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" t="s">
         <v>105</v>
-      </c>
-      <c r="C23" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1086,10 +1092,10 @@
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1097,16 +1103,16 @@
         <v>44</v>
       </c>
       <c r="B25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" t="s">
         <v>107</v>
-      </c>
-      <c r="C25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1114,10 +1120,10 @@
         <v>45</v>
       </c>
       <c r="B26" t="s">
+        <v>123</v>
+      </c>
+      <c r="C26" t="s">
         <v>117</v>
-      </c>
-      <c r="C26" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1125,10 +1131,10 @@
         <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1136,10 +1142,10 @@
         <v>47</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1147,7 +1153,7 @@
         <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
@@ -1155,10 +1161,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
         <v>50</v>
@@ -1166,10 +1172,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
         <v>36</v>
@@ -1186,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1228,7 +1234,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1237,7 +1243,7 @@
         <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -1245,16 +1251,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
@@ -1262,220 +1268,220 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" t="s">
         <v>113</v>
-      </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" t="s">
-        <v>86</v>
-      </c>
-      <c r="G4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" t="s">
         <v>113</v>
-      </c>
-      <c r="C5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" t="s">
         <v>113</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" t="s">
         <v>113</v>
-      </c>
-      <c r="C7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" t="s">
-        <v>89</v>
-      </c>
-      <c r="G7" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" t="s">
         <v>113</v>
-      </c>
-      <c r="C8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" t="s">
         <v>113</v>
-      </c>
-      <c r="C9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" t="s">
         <v>113</v>
-      </c>
-      <c r="C10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G10" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" t="s">
         <v>113</v>
-      </c>
-      <c r="C11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G11" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" t="s">
         <v>113</v>
-      </c>
-      <c r="C12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" t="s">
+        <v>94</v>
+      </c>
+      <c r="G13" t="s">
         <v>113</v>
-      </c>
-      <c r="C13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" t="s">
-        <v>95</v>
-      </c>
-      <c r="G13" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14" t="s">
         <v>113</v>
-      </c>
-      <c r="C14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" t="s">
         <v>113</v>
-      </c>
-      <c r="C15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G15" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G16" t="s">
         <v>8</v>
@@ -1483,16 +1489,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
         <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G17" t="s">
         <v>52</v>
@@ -1500,16 +1506,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
         <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
         <v>52</v>
@@ -1517,16 +1523,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G19" t="s">
         <v>52</v>
@@ -1534,16 +1540,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
         <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G20" t="s">
         <v>52</v>
@@ -1551,16 +1557,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
         <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G21" t="s">
         <v>52</v>
@@ -1568,16 +1574,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
         <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G22" t="s">
         <v>52</v>
@@ -1585,16 +1591,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G23" t="s">
         <v>10</v>
@@ -1602,16 +1608,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
@@ -1619,33 +1625,33 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" t="s">
         <v>58</v>
-      </c>
-      <c r="C25" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B26" t="s">
         <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G26" t="s">
         <v>54</v>
@@ -1653,16 +1659,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G27" t="s">
         <v>10</v>
@@ -1670,69 +1676,86 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D28" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="G28" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="G29" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
         <v>15</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>36</v>
       </c>
-      <c r="D31" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="D32" t="s">
+        <v>62</v>
+      </c>
+      <c r="G32" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update adcore mods and templates
</commit_message>
<xml_diff>
--- a/adcore/2020/templates/2020-super-category.xlsx
+++ b/adcore/2020/templates/2020-super-category.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/11411/Dropbox/git/repo/agency/adcore/2020/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537AE3FF-1B91-4246-BF61-6DEB33BAE949}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3594BD-A2CD-0A45-887E-FA1F6BD12C5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="45780" windowHeight="25500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="131">
   <si>
     <t>Offer Code</t>
   </si>
@@ -228,9 +228,6 @@
     <t>H2</t>
   </si>
   <si>
-    <t>Accordion/Custom List</t>
-  </si>
-  <si>
     <t>Banner 1</t>
   </si>
   <si>
@@ -409,6 +406,24 @@
   </si>
   <si>
     <t>Banner 4</t>
+  </si>
+  <si>
+    <t>Parametric Search</t>
+  </si>
+  <si>
+    <t>WXX_XX_XXX_XXXPS</t>
+  </si>
+  <si>
+    <t>Accordion</t>
+  </si>
+  <si>
+    <t>W21_00_000_UPLDPS</t>
+  </si>
+  <si>
+    <t>BrowseResultsDynTemp</t>
+  </si>
+  <si>
+    <t>Parametric Search/Accordion/Carousel</t>
   </si>
 </sst>
 </file>
@@ -446,7 +461,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -454,13 +469,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,14 +506,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{97FD37EF-440B-164F-A671-9404BC5B49C2}" name="Table2" displayName="Table2" ref="A1:E31" totalsRowShown="0">
-  <autoFilter ref="A1:E31" xr:uid="{46B822AB-FF4E-B747-B408-B19D12290E92}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{97FD37EF-440B-164F-A671-9404BC5B49C2}" name="Table2" displayName="Table2" ref="A1:F31" totalsRowShown="0">
+  <autoFilter ref="A1:F31" xr:uid="{46B822AB-FF4E-B747-B408-B19D12290E92}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{17C01559-4713-534F-9A9B-549B487B8F5A}" name="Module"/>
     <tableColumn id="2" xr3:uid="{FC851083-6D66-B24A-8460-C785CF4AAE2A}" name="Offer Code"/>
     <tableColumn id="3" xr3:uid="{DEC14A67-67A3-0F43-B97F-64C2002A3EBD}" name="Description"/>
+    <tableColumn id="6" xr3:uid="{9B4BA7D4-3222-EB4D-933F-EE64CAD63AA2}" name="Accordion"/>
+    <tableColumn id="5" xr3:uid="{FF53BC05-753C-034B-B16B-9735AEA799A9}" name="Carousel"/>
     <tableColumn id="4" xr3:uid="{CDB8C82C-9162-FA42-B6A8-8BDC4B93A20B}" name="Blank"/>
-    <tableColumn id="5" xr3:uid="{FF53BC05-753C-034B-B16B-9735AEA799A9}" name="Carousel"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -813,22 +841,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -839,13 +869,16 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -856,288 +889,291 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>42</v>
       </c>
       <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" t="s">
         <v>104</v>
       </c>
-      <c r="C23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>44</v>
       </c>
       <c r="B25" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" t="s">
         <v>106</v>
       </c>
-      <c r="C25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" t="s">
-        <v>116</v>
-      </c>
-      <c r="E25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C27" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -1145,10 +1181,10 @@
         <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -1159,9 +1195,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B30" t="s">
         <v>61</v>
@@ -1170,9 +1206,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B31" t="s">
         <v>62</v>
@@ -1192,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1206,7 +1242,7 @@
     <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1251,16 +1287,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
@@ -1268,220 +1304,220 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s">
         <v>112</v>
-      </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
         <v>112</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" t="s">
         <v>112</v>
-      </c>
-      <c r="C6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" t="s">
         <v>112</v>
-      </c>
-      <c r="C7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" t="s">
-        <v>88</v>
-      </c>
-      <c r="G7" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" t="s">
         <v>112</v>
-      </c>
-      <c r="C8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G8" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" t="s">
         <v>112</v>
-      </c>
-      <c r="C9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G9" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" t="s">
         <v>112</v>
-      </c>
-      <c r="C10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G10" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" t="s">
         <v>112</v>
-      </c>
-      <c r="C11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" t="s">
         <v>112</v>
-      </c>
-      <c r="C12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" t="s">
-        <v>93</v>
-      </c>
-      <c r="G12" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" t="s">
         <v>112</v>
-      </c>
-      <c r="C13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" t="s">
-        <v>94</v>
-      </c>
-      <c r="G13" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" t="s">
+        <v>94</v>
+      </c>
+      <c r="G14" t="s">
         <v>112</v>
-      </c>
-      <c r="C14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" t="s">
-        <v>95</v>
-      </c>
-      <c r="G14" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" t="s">
         <v>112</v>
-      </c>
-      <c r="C15" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" t="s">
-        <v>96</v>
-      </c>
-      <c r="G15" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G16" t="s">
         <v>8</v>
@@ -1489,16 +1525,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
         <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G17" t="s">
         <v>52</v>
@@ -1506,16 +1542,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
         <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G18" t="s">
         <v>52</v>
@@ -1523,16 +1559,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
         <v>52</v>
@@ -1540,16 +1576,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
         <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G20" t="s">
         <v>52</v>
@@ -1557,16 +1593,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" t="s">
         <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G21" t="s">
         <v>52</v>
@@ -1574,16 +1610,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
         <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G22" t="s">
         <v>52</v>
@@ -1591,16 +1627,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G23" t="s">
         <v>10</v>
@@ -1608,84 +1644,84 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>106</v>
+      <c r="A25" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
-      </c>
-      <c r="D25" t="s">
-        <v>106</v>
+        <v>125</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="G25" t="s">
-        <v>58</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="D26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G26" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="D27" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="G27" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B28" t="s">
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D28" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="G28" t="s">
         <v>10</v>
@@ -1693,69 +1729,86 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D29" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G29" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>120</v>
       </c>
       <c r="D30" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="G30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>62</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>15</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>36</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>62</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G33" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>